<commit_message>
Update role filtering in count_instructors function and dashboard.html
</commit_message>
<xml_diff>
--- a/static/horarios/1-2024-v3.xlsx
+++ b/static/horarios/1-2024-v3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\schedule\static\horarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{334C9039-774D-4D37-BFAC-3E88C665709A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42462341-8721-4C0E-96FF-A5768740C5D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlcn.WorksheetConnection_CONSOLIDADO_I_2024_V2.xlsxPROGRAMACIONES_PARCIALES" hidden="1">PROGRAMACIONES_PARCIALES[]</definedName>
+    <definedName name="_xlcn.WorksheetConnection_CONSOLIDADO_I_2024_V2.xlsxPROGRAMACIONES_PARCIALES1" hidden="1">PROGRAMACIONES_PARCIALES[]</definedName>
     <definedName name="DatosExternos_1" localSheetId="0" hidden="1">'PROGRAMACIÓN I 2024'!$A$2:$DA$377</definedName>
     <definedName name="SegmentaciónDeDatos_13_14L">#N/A</definedName>
     <definedName name="SegmentaciónDeDatos_19_20L">#N/A</definedName>
@@ -104,7 +104,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="PROGRAMACIONES_PARCIALES" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_CONSOLIDADO_I_2024_V2.xlsxPROGRAMACIONES_PARCIALES"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_CONSOLIDADO_I_2024_V2.xlsxPROGRAMACIONES_PARCIALES1"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2987" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3047" uniqueCount="503">
   <si>
     <t>Source.Name</t>
   </si>
@@ -1324,9 +1324,6 @@
     <t>GESTIONAR PROCESOS PROPIOS DE LA CULTURA EMPRENDEDORAY EMPRESARIA DE ACUERDO CON EL PERFIL PERSONAL Y LOS REQUERIMIENTOS DE LOS CONTEXTOS PRODICTIVO Y SOCIAL - Emprendimiento</t>
   </si>
   <si>
-    <t>2875572 A</t>
-  </si>
-  <si>
     <t>TEC. ELABORACIÓN AUDIOVISUALES</t>
   </si>
   <si>
@@ -1588,6 +1585,15 @@
     <t>2875444 A</t>
   </si>
   <si>
+    <t>2742580 C</t>
+  </si>
+  <si>
+    <t>TEC303</t>
+  </si>
+  <si>
+    <t>2875586 A</t>
+  </si>
+  <si>
     <t>6-7S</t>
   </si>
   <si>
@@ -1616,9 +1622,6 @@
   </si>
   <si>
     <t>21-22S</t>
-  </si>
-  <si>
-    <t>2742580 C</t>
   </si>
 </sst>
 </file>
@@ -1688,7 +1691,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1704,6 +1707,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2571,11 +2575,6 @@
       <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
   <c:extLst>
     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{723BEF56-08C2-4564-9609-F4CBC75E7E54}">
       <c15:pivotSource>
@@ -4987,231 +4986,6 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3EA41CB7-E3A8-430F-B4AE-F3DE60532250}" name="TablaDinámica3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="D30:E47" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="2">
-    <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1">
-      <items count="16">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="17">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Recuento distinto de FICHA" fld="1" subtotal="count" baseField="0" baseItem="0">
-      <extLst>
-        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{FABC7310-3BB5-11E1-824E-6D434824019B}">
-          <x15:dataField isCountDistinct="1"/>
-        </ext>
-      </extLst>
-    </dataField>
-  </dataFields>
-  <pivotHierarchies count="109">
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1" caption="Recuento distinto de FICHA"/>
-  </pivotHierarchies>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <rowHierarchiesUsage count="1">
-    <rowHierarchyUsage hierarchyUsage="2"/>
-  </rowHierarchiesUsage>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" calculatedMembersInFilters="1" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{E67621CE-5B39-4880-91FE-76760E9C1902}">
-      <x15:pivotTableUISettings sourceDataName="WorksheetConnection_CONSOLIDADO_I_2024_V2.xlsx!PROGRAMACIONES_PARCIALES">
-        <x15:activeTabTopLevelEntity name="[PROGRAMACIONES_PARCIALES]"/>
-      </x15:pivotTableUISettings>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E51D2C13-18A8-44E4-9514-17D00C659F63}" name="TablaDinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B82" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
@@ -5661,6 +5435,231 @@
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <rowHierarchiesUsage count="1">
     <rowHierarchyUsage hierarchyUsage="13"/>
+  </rowHierarchiesUsage>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" calculatedMembersInFilters="1" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{E67621CE-5B39-4880-91FE-76760E9C1902}">
+      <x15:pivotTableUISettings sourceDataName="WorksheetConnection_CONSOLIDADO_I_2024_V2.xlsx!PROGRAMACIONES_PARCIALES">
+        <x15:activeTabTopLevelEntity name="[PROGRAMACIONES_PARCIALES]"/>
+      </x15:pivotTableUISettings>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3EA41CB7-E3A8-430F-B4AE-F3DE60532250}" name="TablaDinámica3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="D30:E47" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1">
+      <items count="16">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="17">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Recuento distinto de FICHA" fld="1" subtotal="count" baseField="0" baseItem="0">
+      <extLst>
+        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{FABC7310-3BB5-11E1-824E-6D434824019B}">
+          <x15:dataField isCountDistinct="1"/>
+        </ext>
+      </extLst>
+    </dataField>
+  </dataFields>
+  <pivotHierarchies count="109">
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1" caption="Recuento distinto de FICHA"/>
+  </pivotHierarchies>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <rowHierarchiesUsage count="1">
+    <rowHierarchyUsage hierarchyUsage="2"/>
   </rowHierarchiesUsage>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -6108,7 +6107,7 @@
     <tableColumn id="97" xr3:uid="{C47FF5A8-51B9-41AF-8D63-CEB7C92ACB49}" uniqueName="97" name="21-22V" totalsRowFunction="custom" queryTableFieldId="97">
       <totalsRowFormula>SUBTOTAL(3,PROGRAMACIONES_PARCIALES[21-22V])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{DD845AE9-38B6-4A80-8432-09E4AAC72E7D}" uniqueName="1" name="6-7S" queryTableFieldId="105"/>
+    <tableColumn id="1" xr3:uid="{DA68D4F0-B1F1-4D08-8BBA-5EE8F6703898}" uniqueName="1" name="6-7S" queryTableFieldId="105"/>
     <tableColumn id="98" xr3:uid="{25044A8C-0253-4E22-980E-977A3B5C6C59}" uniqueName="98" name="7-8S" totalsRowFunction="custom" queryTableFieldId="98">
       <totalsRowFormula>SUBTOTAL(3,PROGRAMACIONES_PARCIALES[7-8S])</totalsRowFormula>
     </tableColumn>
@@ -6130,14 +6129,14 @@
     <tableColumn id="104" xr3:uid="{FD79054B-1F48-4B17-8E3F-E8071CD3F12B}" uniqueName="104" name="13-14S" totalsRowFunction="custom" queryTableFieldId="104">
       <totalsRowFormula>SUBTOTAL(3,PROGRAMACIONES_PARCIALES[13-14S])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="106" xr3:uid="{F040B160-123F-41F3-833E-B05E986C4DBF}" uniqueName="106" name="14-15S" queryTableFieldId="106"/>
-    <tableColumn id="107" xr3:uid="{10D02C96-E34A-4B40-8233-841B3C266A70}" uniqueName="107" name="15-16S" queryTableFieldId="107"/>
-    <tableColumn id="108" xr3:uid="{D5E03B02-FE6E-48D4-A664-5FAA42BACB7D}" uniqueName="108" name="16-17S" queryTableFieldId="108"/>
-    <tableColumn id="109" xr3:uid="{758A1885-478F-4515-9C8C-DF421652753D}" uniqueName="109" name="17-18S" queryTableFieldId="109"/>
-    <tableColumn id="110" xr3:uid="{9CCED529-3CAC-460F-AD3A-DD847BD4918E}" uniqueName="110" name="18-19S" queryTableFieldId="110"/>
-    <tableColumn id="111" xr3:uid="{ED6351E4-53CD-42B7-8B6E-E94C6269E09D}" uniqueName="111" name="19-20S" queryTableFieldId="111"/>
-    <tableColumn id="112" xr3:uid="{018626A8-6BC4-4D1A-AF55-EB05137C4C4C}" uniqueName="112" name="20-21S" queryTableFieldId="112"/>
-    <tableColumn id="113" xr3:uid="{DA218E77-EC56-4B52-B643-4E7D054D4396}" uniqueName="113" name="21-22S" queryTableFieldId="113"/>
+    <tableColumn id="106" xr3:uid="{F7C9ADE6-EB7A-429A-8C5A-DB58B52CA8BD}" uniqueName="106" name="14-15S" queryTableFieldId="106"/>
+    <tableColumn id="107" xr3:uid="{C0F52894-9EE5-45F0-8371-0D086A3E656E}" uniqueName="107" name="15-16S" queryTableFieldId="107"/>
+    <tableColumn id="108" xr3:uid="{241E9FC5-1B0A-43B4-842D-347B3CB21248}" uniqueName="108" name="16-17S" queryTableFieldId="108"/>
+    <tableColumn id="109" xr3:uid="{DB43EF92-8B09-47AF-AEC7-A29A0EF9AAC6}" uniqueName="109" name="17-18S" queryTableFieldId="109"/>
+    <tableColumn id="110" xr3:uid="{1DD59851-2B16-49E1-9997-DE25D84F36D4}" uniqueName="110" name="18-19S" queryTableFieldId="110"/>
+    <tableColumn id="111" xr3:uid="{9921D150-7286-485E-A9EE-60E5572AC3E4}" uniqueName="111" name="19-20S" queryTableFieldId="111"/>
+    <tableColumn id="112" xr3:uid="{8D7D2FF1-C4A3-4428-8658-87BE8379F37F}" uniqueName="112" name="20-21S" queryTableFieldId="112"/>
+    <tableColumn id="113" xr3:uid="{4E35FCDC-686A-4555-AD55-FB43AD30547C}" uniqueName="113" name="21-22S" queryTableFieldId="113"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6413,10 +6412,10 @@
 </file>
 
 <file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{3C9AC298-184D-4F56-A345-DA071939C279}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{160A34EE-E4AE-446D-B0BE-F0187B8A3549}">
   <we:reference id="wa104380263" version="1.1.3.0" store="es-ES" storeType="OMEX"/>
   <we:alternateReferences>
-    <we:reference id="WA104380263" version="1.1.3.0" store="WA104380263" storeType="OMEX"/>
+    <we:reference id="wa104380263" version="1.1.3.0" store="WA104380263" storeType="OMEX"/>
   </we:alternateReferences>
   <we:properties/>
   <we:bindings/>
@@ -6428,8 +6427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C46E5B-3CE7-4F67-9F7E-3BDF34AAB992}">
   <dimension ref="A1:DI378"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A164" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C178" sqref="C178"/>
+    <sheetView tabSelected="1" topLeftCell="CJ353" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:DI377"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6470,10 +6469,10 @@
     <row r="1" spans="1:113" ht="118.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="P1" s="1">
         <f>SUBTOTAL(9,PROGRAMACIONES_PARCIALES[HORAS SEMANAL])</f>
-        <v>2042</v>
+        <v>2044</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="S1" s="6"/>
       <c r="T1" s="6"/>
@@ -6491,7 +6490,7 @@
       <c r="AF1" s="6"/>
       <c r="AG1" s="6"/>
       <c r="AH1" s="6" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="AI1" s="6"/>
       <c r="AJ1" s="6"/>
@@ -6509,7 +6508,7 @@
       <c r="AV1" s="6"/>
       <c r="AW1" s="6"/>
       <c r="AX1" s="6" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="AY1" s="6"/>
       <c r="AZ1" s="6"/>
@@ -6527,7 +6526,7 @@
       <c r="BL1" s="6"/>
       <c r="BM1" s="6"/>
       <c r="BN1" s="6" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="BO1" s="6"/>
       <c r="BP1" s="6"/>
@@ -6545,7 +6544,7 @@
       <c r="CB1" s="6"/>
       <c r="CC1" s="6"/>
       <c r="CD1" s="6" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="CE1" s="6"/>
       <c r="CF1" s="6"/>
@@ -6564,7 +6563,7 @@
       <c r="CS1" s="6"/>
       <c r="CT1" s="5"/>
       <c r="CU1" s="6" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="CV1" s="6"/>
       <c r="CW1" s="6"/>
@@ -6865,53 +6864,53 @@
       <c r="CS2" t="s">
         <v>96</v>
       </c>
-      <c r="CT2" t="s">
-        <v>491</v>
-      </c>
-      <c r="CU2" t="s">
-        <v>492</v>
-      </c>
-      <c r="CV2" t="s">
+      <c r="CT2" s="7" t="s">
+        <v>493</v>
+      </c>
+      <c r="CU2" s="7" t="s">
+        <v>494</v>
+      </c>
+      <c r="CV2" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="CW2" t="s">
+      <c r="CW2" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="CX2" t="s">
+      <c r="CX2" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="CY2" t="s">
+      <c r="CY2" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="CZ2" t="s">
+      <c r="CZ2" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="DA2" t="s">
+      <c r="DA2" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="DB2" t="s">
-        <v>493</v>
-      </c>
-      <c r="DC2" t="s">
-        <v>494</v>
-      </c>
-      <c r="DD2" t="s">
+      <c r="DB2" s="7" t="s">
         <v>495</v>
       </c>
-      <c r="DE2" t="s">
+      <c r="DC2" s="7" t="s">
         <v>496</v>
       </c>
-      <c r="DF2" t="s">
+      <c r="DD2" s="7" t="s">
         <v>497</v>
       </c>
-      <c r="DG2" t="s">
+      <c r="DE2" s="7" t="s">
         <v>498</v>
       </c>
-      <c r="DH2" t="s">
+      <c r="DF2" s="7" t="s">
         <v>499</v>
       </c>
-      <c r="DI2" t="s">
+      <c r="DG2" s="7" t="s">
         <v>500</v>
+      </c>
+      <c r="DH2" s="7" t="s">
+        <v>501</v>
+      </c>
+      <c r="DI2" s="7" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="3" spans="1:113" x14ac:dyDescent="0.3">
@@ -7517,7 +7516,7 @@
         <v>1</v>
       </c>
       <c r="N11" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="P11">
         <v>2</v>
@@ -7718,7 +7717,7 @@
         <v>1</v>
       </c>
       <c r="N14" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="P14">
         <v>2</v>
@@ -7969,7 +7968,7 @@
         <v>1</v>
       </c>
       <c r="N18" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="P18">
         <v>2</v>
@@ -8146,7 +8145,7 @@
         <v>1</v>
       </c>
       <c r="N21" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="P21">
         <v>2</v>
@@ -8246,7 +8245,7 @@
         <v>1</v>
       </c>
       <c r="N23" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="P23">
         <v>2</v>
@@ -8337,7 +8336,7 @@
         <v>1</v>
       </c>
       <c r="N25" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="P25">
         <v>2</v>
@@ -8918,7 +8917,7 @@
         <v>1</v>
       </c>
       <c r="N35" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="P35">
         <v>2</v>
@@ -9011,65 +9010,65 @@
       <c r="Q37">
         <v>240</v>
       </c>
-      <c r="Z37">
-        <v>4</v>
-      </c>
-      <c r="AA37">
-        <v>4</v>
-      </c>
-      <c r="AB37">
-        <v>4</v>
-      </c>
-      <c r="AC37">
-        <v>4</v>
-      </c>
-      <c r="AP37">
-        <v>4</v>
-      </c>
-      <c r="AQ37">
-        <v>4</v>
-      </c>
-      <c r="AR37">
-        <v>4</v>
-      </c>
-      <c r="AS37">
-        <v>4</v>
-      </c>
-      <c r="BD37">
-        <v>4</v>
-      </c>
-      <c r="BE37">
-        <v>4</v>
-      </c>
-      <c r="BF37">
-        <v>4</v>
-      </c>
-      <c r="BG37">
-        <v>4</v>
-      </c>
-      <c r="BV37">
-        <v>4</v>
-      </c>
-      <c r="BW37">
-        <v>4</v>
-      </c>
-      <c r="BX37">
-        <v>4</v>
-      </c>
-      <c r="BY37">
-        <v>4</v>
-      </c>
-      <c r="CL37">
-        <v>4</v>
-      </c>
-      <c r="CM37">
-        <v>4</v>
-      </c>
-      <c r="CN37">
-        <v>4</v>
-      </c>
-      <c r="CO37">
-        <v>4</v>
+      <c r="Z37" t="s">
+        <v>491</v>
+      </c>
+      <c r="AA37" t="s">
+        <v>491</v>
+      </c>
+      <c r="AB37" t="s">
+        <v>491</v>
+      </c>
+      <c r="AC37" t="s">
+        <v>491</v>
+      </c>
+      <c r="AP37" t="s">
+        <v>491</v>
+      </c>
+      <c r="AQ37" t="s">
+        <v>491</v>
+      </c>
+      <c r="AR37" t="s">
+        <v>491</v>
+      </c>
+      <c r="AS37" t="s">
+        <v>491</v>
+      </c>
+      <c r="BD37" t="s">
+        <v>491</v>
+      </c>
+      <c r="BE37" t="s">
+        <v>491</v>
+      </c>
+      <c r="BF37" t="s">
+        <v>491</v>
+      </c>
+      <c r="BG37" t="s">
+        <v>491</v>
+      </c>
+      <c r="BV37" t="s">
+        <v>491</v>
+      </c>
+      <c r="BW37" t="s">
+        <v>491</v>
+      </c>
+      <c r="BX37" t="s">
+        <v>491</v>
+      </c>
+      <c r="BY37" t="s">
+        <v>491</v>
+      </c>
+      <c r="CL37" t="s">
+        <v>491</v>
+      </c>
+      <c r="CM37" t="s">
+        <v>491</v>
+      </c>
+      <c r="CN37" t="s">
+        <v>491</v>
+      </c>
+      <c r="CO37" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="38" spans="1:105" x14ac:dyDescent="0.3">
@@ -9115,11 +9114,11 @@
       <c r="Q38">
         <v>24</v>
       </c>
-      <c r="X38">
-        <v>4</v>
-      </c>
-      <c r="Y38">
-        <v>4</v>
+      <c r="X38" t="s">
+        <v>491</v>
+      </c>
+      <c r="Y38" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="39" spans="1:105" x14ac:dyDescent="0.3">
@@ -9165,11 +9164,11 @@
       <c r="Q39">
         <v>24</v>
       </c>
-      <c r="AN39">
-        <v>4</v>
-      </c>
-      <c r="AO39">
-        <v>4</v>
+      <c r="AN39" t="s">
+        <v>491</v>
+      </c>
+      <c r="AO39" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="40" spans="1:105" x14ac:dyDescent="0.3">
@@ -9215,11 +9214,11 @@
       <c r="Q40">
         <v>24</v>
       </c>
-      <c r="BH40">
-        <v>4</v>
-      </c>
-      <c r="BI40">
-        <v>4</v>
+      <c r="BH40" t="s">
+        <v>491</v>
+      </c>
+      <c r="BI40" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="41" spans="1:105" x14ac:dyDescent="0.3">
@@ -9265,11 +9264,11 @@
       <c r="Q41">
         <v>24</v>
       </c>
-      <c r="CJ41">
-        <v>4</v>
-      </c>
-      <c r="CK41">
-        <v>4</v>
+      <c r="CJ41" t="s">
+        <v>491</v>
+      </c>
+      <c r="CK41" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="42" spans="1:105" x14ac:dyDescent="0.3">
@@ -9306,11 +9305,11 @@
       <c r="Q42">
         <v>24</v>
       </c>
-      <c r="BT42">
-        <v>4</v>
-      </c>
-      <c r="BU42">
-        <v>4</v>
+      <c r="BT42" t="s">
+        <v>491</v>
+      </c>
+      <c r="BU42" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="43" spans="1:105" x14ac:dyDescent="0.3">
@@ -9932,7 +9931,7 @@
         <v>1</v>
       </c>
       <c r="N53" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="P53">
         <v>2</v>
@@ -10098,7 +10097,7 @@
         <v>1</v>
       </c>
       <c r="N55" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="P55">
         <v>2</v>
@@ -10422,7 +10421,7 @@
         <v>1</v>
       </c>
       <c r="N61" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="P61">
         <v>2</v>
@@ -10743,7 +10742,7 @@
         <v>1</v>
       </c>
       <c r="N67" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="P67">
         <v>2</v>
@@ -10793,7 +10792,7 @@
         <v>1</v>
       </c>
       <c r="N68" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="P68">
         <v>2</v>
@@ -10936,77 +10935,77 @@
       <c r="Q71">
         <v>288</v>
       </c>
-      <c r="R71">
-        <v>4</v>
-      </c>
-      <c r="S71">
-        <v>4</v>
-      </c>
-      <c r="T71">
-        <v>4</v>
-      </c>
-      <c r="U71">
-        <v>4</v>
-      </c>
-      <c r="AH71">
-        <v>4</v>
-      </c>
-      <c r="AI71">
-        <v>4</v>
-      </c>
-      <c r="AJ71">
-        <v>4</v>
-      </c>
-      <c r="AK71">
-        <v>4</v>
-      </c>
-      <c r="AL71">
-        <v>4</v>
-      </c>
-      <c r="AM71">
-        <v>4</v>
-      </c>
-      <c r="AX71">
-        <v>4</v>
-      </c>
-      <c r="AY71">
-        <v>4</v>
-      </c>
-      <c r="AZ71">
-        <v>4</v>
-      </c>
-      <c r="BA71">
-        <v>4</v>
-      </c>
-      <c r="BB71">
-        <v>4</v>
-      </c>
-      <c r="BC71">
-        <v>4</v>
-      </c>
-      <c r="BN71">
-        <v>4</v>
-      </c>
-      <c r="BO71">
-        <v>4</v>
-      </c>
-      <c r="BP71">
-        <v>4</v>
-      </c>
-      <c r="BQ71">
-        <v>4</v>
-      </c>
-      <c r="CD71">
-        <v>4</v>
-      </c>
-      <c r="CE71">
-        <v>4</v>
-      </c>
-      <c r="CF71">
-        <v>4</v>
-      </c>
-      <c r="CG71">
-        <v>4</v>
+      <c r="R71" t="s">
+        <v>491</v>
+      </c>
+      <c r="S71" t="s">
+        <v>491</v>
+      </c>
+      <c r="T71" t="s">
+        <v>491</v>
+      </c>
+      <c r="U71" t="s">
+        <v>491</v>
+      </c>
+      <c r="AH71" t="s">
+        <v>491</v>
+      </c>
+      <c r="AI71" t="s">
+        <v>491</v>
+      </c>
+      <c r="AJ71" t="s">
+        <v>491</v>
+      </c>
+      <c r="AK71" t="s">
+        <v>491</v>
+      </c>
+      <c r="AL71" t="s">
+        <v>491</v>
+      </c>
+      <c r="AM71" t="s">
+        <v>491</v>
+      </c>
+      <c r="AX71" t="s">
+        <v>491</v>
+      </c>
+      <c r="AY71" t="s">
+        <v>491</v>
+      </c>
+      <c r="AZ71" t="s">
+        <v>491</v>
+      </c>
+      <c r="BA71" t="s">
+        <v>491</v>
+      </c>
+      <c r="BB71" t="s">
+        <v>491</v>
+      </c>
+      <c r="BC71" t="s">
+        <v>491</v>
+      </c>
+      <c r="BN71" t="s">
+        <v>491</v>
+      </c>
+      <c r="BO71" t="s">
+        <v>491</v>
+      </c>
+      <c r="BP71" t="s">
+        <v>491</v>
+      </c>
+      <c r="BQ71" t="s">
+        <v>491</v>
+      </c>
+      <c r="CD71" t="s">
+        <v>491</v>
+      </c>
+      <c r="CE71" t="s">
+        <v>491</v>
+      </c>
+      <c r="CF71" t="s">
+        <v>491</v>
+      </c>
+      <c r="CG71" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="72" spans="1:105" x14ac:dyDescent="0.3">
@@ -11052,11 +11051,11 @@
       <c r="Q72">
         <v>24</v>
       </c>
-      <c r="BR72">
-        <v>4</v>
-      </c>
-      <c r="BS72">
-        <v>4</v>
+      <c r="BR72" t="s">
+        <v>491</v>
+      </c>
+      <c r="BS72" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="73" spans="1:105" x14ac:dyDescent="0.3">
@@ -11102,11 +11101,11 @@
       <c r="Q73">
         <v>24</v>
       </c>
-      <c r="CH73">
-        <v>4</v>
-      </c>
-      <c r="CI73">
-        <v>4</v>
+      <c r="CH73" t="s">
+        <v>491</v>
+      </c>
+      <c r="CI73" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="74" spans="1:105" x14ac:dyDescent="0.3">
@@ -11143,11 +11142,11 @@
       <c r="Q74">
         <v>24</v>
       </c>
-      <c r="V74">
-        <v>4</v>
-      </c>
-      <c r="W74">
-        <v>4</v>
+      <c r="V74" t="s">
+        <v>491</v>
+      </c>
+      <c r="W74" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="75" spans="1:105" x14ac:dyDescent="0.3">
@@ -11456,7 +11455,7 @@
         <v>103</v>
       </c>
       <c r="B80" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C80" t="s">
         <v>105</v>
@@ -11500,7 +11499,7 @@
         <v>103</v>
       </c>
       <c r="B81" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C81" t="s">
         <v>105</v>
@@ -11622,7 +11621,7 @@
         <v>103</v>
       </c>
       <c r="B82" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C82" t="s">
         <v>105</v>
@@ -11663,7 +11662,7 @@
         <v>103</v>
       </c>
       <c r="B83" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C83" t="s">
         <v>105</v>
@@ -11713,7 +11712,7 @@
         <v>103</v>
       </c>
       <c r="B84" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C84" t="s">
         <v>105</v>
@@ -11745,7 +11744,7 @@
         <v>103</v>
       </c>
       <c r="B85" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C85" t="s">
         <v>105</v>
@@ -11867,7 +11866,7 @@
         <v>103</v>
       </c>
       <c r="B86" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C86" t="s">
         <v>105</v>
@@ -11917,7 +11916,7 @@
         <v>103</v>
       </c>
       <c r="B87" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C87" t="s">
         <v>105</v>
@@ -11938,7 +11937,7 @@
         <v>1</v>
       </c>
       <c r="N87" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="P87">
         <v>2</v>
@@ -12851,7 +12850,7 @@
         <v>1</v>
       </c>
       <c r="N104" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="O104" t="s">
         <v>195</v>
@@ -13502,7 +13501,7 @@
         <v>1</v>
       </c>
       <c r="N116" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="O116" t="s">
         <v>215</v>
@@ -15568,7 +15567,7 @@
         <v>1</v>
       </c>
       <c r="N153" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="O153" t="s">
         <v>195</v>
@@ -16164,7 +16163,7 @@
         <v>1</v>
       </c>
       <c r="N163" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="O163" t="s">
         <v>195</v>
@@ -16365,7 +16364,7 @@
         <v>1</v>
       </c>
       <c r="N166" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="O166" t="s">
         <v>255</v>
@@ -17119,7 +17118,7 @@
         <v>184</v>
       </c>
       <c r="B180" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
       <c r="C180" t="s">
         <v>186</v>
@@ -17175,7 +17174,7 @@
         <v>184</v>
       </c>
       <c r="B181" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
       <c r="C181" t="s">
         <v>186</v>
@@ -17228,7 +17227,7 @@
         <v>184</v>
       </c>
       <c r="B182" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
       <c r="C182" t="s">
         <v>186</v>
@@ -17305,7 +17304,7 @@
         <v>184</v>
       </c>
       <c r="B183" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
       <c r="C183" t="s">
         <v>186</v>
@@ -17358,7 +17357,7 @@
         <v>184</v>
       </c>
       <c r="B184" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
       <c r="C184" t="s">
         <v>186</v>
@@ -17411,7 +17410,7 @@
         <v>184</v>
       </c>
       <c r="B185" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
       <c r="C185" t="s">
         <v>186</v>
@@ -17715,7 +17714,7 @@
         <v>1</v>
       </c>
       <c r="N190" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="O190" t="s">
         <v>215</v>
@@ -18036,7 +18035,7 @@
         <v>1</v>
       </c>
       <c r="N196" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="O196" t="s">
         <v>195</v>
@@ -18410,7 +18409,7 @@
         <v>1</v>
       </c>
       <c r="N203" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="O203" t="s">
         <v>195</v>
@@ -19099,7 +19098,7 @@
         <v>1</v>
       </c>
       <c r="N216" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="O216" t="s">
         <v>195</v>
@@ -20585,7 +20584,7 @@
         <v>1</v>
       </c>
       <c r="N242" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="P242">
         <v>2</v>
@@ -20685,7 +20684,7 @@
         <v>1</v>
       </c>
       <c r="N244" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="P244">
         <v>2</v>
@@ -22657,7 +22656,7 @@
         <v>1</v>
       </c>
       <c r="N282" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="P282">
         <v>2</v>
@@ -22707,7 +22706,7 @@
         <v>1</v>
       </c>
       <c r="N283" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="P283">
         <v>2</v>
@@ -22917,7 +22916,7 @@
         <v>1</v>
       </c>
       <c r="N286" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="P286">
         <v>2</v>
@@ -24095,7 +24094,7 @@
         <v>1</v>
       </c>
       <c r="N305" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="P305">
         <v>2</v>
@@ -24685,13 +24684,13 @@
         <v>361</v>
       </c>
       <c r="B315" t="s">
+        <v>492</v>
+      </c>
+      <c r="C315" t="s">
         <v>403</v>
       </c>
-      <c r="C315" t="s">
+      <c r="D315" t="s">
         <v>404</v>
-      </c>
-      <c r="D315" t="s">
-        <v>405</v>
       </c>
       <c r="E315">
         <v>1</v>
@@ -24700,7 +24699,7 @@
         <v>216</v>
       </c>
       <c r="G315" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="H315">
         <v>1</v>
@@ -24712,7 +24711,7 @@
         <v>1</v>
       </c>
       <c r="N315" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="P315">
         <v>4</v>
@@ -24738,13 +24737,13 @@
         <v>361</v>
       </c>
       <c r="B316" t="s">
+        <v>492</v>
+      </c>
+      <c r="C316" t="s">
         <v>403</v>
       </c>
-      <c r="C316" t="s">
+      <c r="D316" t="s">
         <v>404</v>
-      </c>
-      <c r="D316" t="s">
-        <v>405</v>
       </c>
       <c r="E316">
         <v>1</v>
@@ -24753,7 +24752,7 @@
         <v>262</v>
       </c>
       <c r="G316" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="H316">
         <v>1</v>
@@ -24768,7 +24767,7 @@
         <v>1</v>
       </c>
       <c r="N316" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="P316">
         <v>20</v>
@@ -24842,13 +24841,13 @@
         <v>361</v>
       </c>
       <c r="B317" t="s">
+        <v>492</v>
+      </c>
+      <c r="C317" t="s">
         <v>403</v>
       </c>
-      <c r="C317" t="s">
+      <c r="D317" t="s">
         <v>404</v>
-      </c>
-      <c r="D317" t="s">
-        <v>405</v>
       </c>
       <c r="E317">
         <v>1</v>
@@ -24892,13 +24891,13 @@
         <v>361</v>
       </c>
       <c r="B318" t="s">
+        <v>492</v>
+      </c>
+      <c r="C318" t="s">
         <v>403</v>
       </c>
-      <c r="C318" t="s">
+      <c r="D318" t="s">
         <v>404</v>
-      </c>
-      <c r="D318" t="s">
-        <v>405</v>
       </c>
       <c r="E318">
         <v>1</v>
@@ -24922,7 +24921,7 @@
         <v>1</v>
       </c>
       <c r="N318" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="P318">
         <v>2</v>
@@ -24942,13 +24941,13 @@
         <v>361</v>
       </c>
       <c r="B319" t="s">
+        <v>492</v>
+      </c>
+      <c r="C319" t="s">
         <v>403</v>
       </c>
-      <c r="C319" t="s">
+      <c r="D319" t="s">
         <v>404</v>
-      </c>
-      <c r="D319" t="s">
-        <v>405</v>
       </c>
       <c r="E319">
         <v>1</v>
@@ -24992,13 +24991,13 @@
         <v>361</v>
       </c>
       <c r="B320" t="s">
+        <v>407</v>
+      </c>
+      <c r="C320" t="s">
         <v>408</v>
       </c>
-      <c r="C320" t="s">
+      <c r="D320" t="s">
         <v>409</v>
-      </c>
-      <c r="D320" t="s">
-        <v>410</v>
       </c>
       <c r="E320">
         <v>1</v>
@@ -25007,7 +25006,7 @@
         <v>216</v>
       </c>
       <c r="G320" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="H320">
         <v>1</v>
@@ -25019,7 +25018,7 @@
         <v>1</v>
       </c>
       <c r="N320" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="P320">
         <v>4</v>
@@ -25045,13 +25044,13 @@
         <v>361</v>
       </c>
       <c r="B321" t="s">
+        <v>407</v>
+      </c>
+      <c r="C321" t="s">
         <v>408</v>
       </c>
-      <c r="C321" t="s">
+      <c r="D321" t="s">
         <v>409</v>
-      </c>
-      <c r="D321" t="s">
-        <v>410</v>
       </c>
       <c r="E321">
         <v>1</v>
@@ -25060,7 +25059,7 @@
         <v>233</v>
       </c>
       <c r="G321" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H321">
         <v>1</v>
@@ -25075,7 +25074,7 @@
         <v>1</v>
       </c>
       <c r="N321" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="P321">
         <v>22</v>
@@ -25155,13 +25154,13 @@
         <v>361</v>
       </c>
       <c r="B322" t="s">
+        <v>407</v>
+      </c>
+      <c r="C322" t="s">
         <v>408</v>
       </c>
-      <c r="C322" t="s">
+      <c r="D322" t="s">
         <v>409</v>
-      </c>
-      <c r="D322" t="s">
-        <v>410</v>
       </c>
       <c r="E322">
         <v>1</v>
@@ -25211,13 +25210,13 @@
         <v>361</v>
       </c>
       <c r="B323" t="s">
+        <v>407</v>
+      </c>
+      <c r="C323" t="s">
         <v>408</v>
       </c>
-      <c r="C323" t="s">
+      <c r="D323" t="s">
         <v>409</v>
-      </c>
-      <c r="D323" t="s">
-        <v>410</v>
       </c>
       <c r="E323">
         <v>1</v>
@@ -25258,16 +25257,16 @@
     </row>
     <row r="324" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
+        <v>411</v>
+      </c>
+      <c r="B324" t="s">
         <v>412</v>
       </c>
-      <c r="B324" t="s">
+      <c r="C324" t="s">
         <v>413</v>
       </c>
-      <c r="C324" t="s">
+      <c r="D324" t="s">
         <v>414</v>
-      </c>
-      <c r="D324" t="s">
-        <v>415</v>
       </c>
       <c r="E324">
         <v>3</v>
@@ -25276,13 +25275,13 @@
         <v>112</v>
       </c>
       <c r="G324" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="J324">
         <v>3</v>
       </c>
       <c r="N324" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="P324">
         <v>8</v>
@@ -25317,16 +25316,16 @@
     </row>
     <row r="325" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
+        <v>411</v>
+      </c>
+      <c r="B325" t="s">
         <v>412</v>
       </c>
-      <c r="B325" t="s">
+      <c r="C325" t="s">
         <v>413</v>
       </c>
-      <c r="C325" t="s">
+      <c r="D325" t="s">
         <v>414</v>
-      </c>
-      <c r="D325" t="s">
-        <v>415</v>
       </c>
       <c r="E325">
         <v>3</v>
@@ -25335,13 +25334,13 @@
         <v>132</v>
       </c>
       <c r="G325" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="J325">
         <v>3</v>
       </c>
       <c r="N325" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="P325">
         <v>4</v>
@@ -25364,16 +25363,16 @@
     </row>
     <row r="326" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
+        <v>411</v>
+      </c>
+      <c r="B326" t="s">
         <v>412</v>
       </c>
-      <c r="B326" t="s">
+      <c r="C326" t="s">
         <v>413</v>
       </c>
-      <c r="C326" t="s">
+      <c r="D326" t="s">
         <v>414</v>
-      </c>
-      <c r="D326" t="s">
-        <v>415</v>
       </c>
       <c r="E326">
         <v>4</v>
@@ -25382,7 +25381,7 @@
         <v>251</v>
       </c>
       <c r="G326" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H326">
         <v>3</v>
@@ -25397,7 +25396,7 @@
         <v>3</v>
       </c>
       <c r="N326" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="P326">
         <v>4</v>
@@ -25420,16 +25419,16 @@
     </row>
     <row r="327" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
+        <v>411</v>
+      </c>
+      <c r="B327" t="s">
         <v>412</v>
       </c>
-      <c r="B327" t="s">
+      <c r="C327" t="s">
         <v>413</v>
       </c>
-      <c r="C327" t="s">
+      <c r="D327" t="s">
         <v>414</v>
-      </c>
-      <c r="D327" t="s">
-        <v>415</v>
       </c>
       <c r="E327">
         <v>3</v>
@@ -25438,13 +25437,13 @@
         <v>264</v>
       </c>
       <c r="G327" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="K327">
         <v>3</v>
       </c>
       <c r="N327" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="P327">
         <v>6</v>
@@ -25473,16 +25472,16 @@
     </row>
     <row r="328" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
+        <v>411</v>
+      </c>
+      <c r="B328" t="s">
         <v>412</v>
       </c>
-      <c r="B328" t="s">
+      <c r="C328" t="s">
         <v>413</v>
       </c>
-      <c r="C328" t="s">
+      <c r="D328" t="s">
         <v>414</v>
-      </c>
-      <c r="D328" t="s">
-        <v>415</v>
       </c>
       <c r="E328">
         <v>3</v>
@@ -25523,16 +25522,16 @@
     </row>
     <row r="329" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
+        <v>411</v>
+      </c>
+      <c r="B329" t="s">
         <v>412</v>
       </c>
-      <c r="B329" t="s">
+      <c r="C329" t="s">
         <v>413</v>
       </c>
-      <c r="C329" t="s">
+      <c r="D329" t="s">
         <v>414</v>
-      </c>
-      <c r="D329" t="s">
-        <v>415</v>
       </c>
       <c r="E329">
         <v>3</v>
@@ -25567,16 +25566,16 @@
     </row>
     <row r="330" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
+        <v>411</v>
+      </c>
+      <c r="B330" t="s">
         <v>412</v>
       </c>
-      <c r="B330" t="s">
+      <c r="C330" t="s">
         <v>413</v>
       </c>
-      <c r="C330" t="s">
+      <c r="D330" t="s">
         <v>414</v>
-      </c>
-      <c r="D330" t="s">
-        <v>415</v>
       </c>
       <c r="E330">
         <v>3</v>
@@ -25585,7 +25584,7 @@
         <v>254</v>
       </c>
       <c r="G330" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H330">
         <v>3</v>
@@ -25600,7 +25599,7 @@
         <v>3</v>
       </c>
       <c r="N330" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="P330">
         <v>2</v>
@@ -25617,25 +25616,25 @@
     </row>
     <row r="331" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
+        <v>411</v>
+      </c>
+      <c r="B331" t="s">
         <v>412</v>
       </c>
-      <c r="B331" t="s">
+      <c r="C331" t="s">
         <v>413</v>
       </c>
-      <c r="C331" t="s">
+      <c r="D331" t="s">
         <v>414</v>
-      </c>
-      <c r="D331" t="s">
-        <v>415</v>
       </c>
       <c r="E331">
         <v>3</v>
       </c>
       <c r="F331" t="s">
+        <v>422</v>
+      </c>
+      <c r="G331" t="s">
         <v>423</v>
-      </c>
-      <c r="G331" t="s">
-        <v>424</v>
       </c>
       <c r="H331">
         <v>3</v>
@@ -25667,16 +25666,16 @@
     </row>
     <row r="332" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B332" t="s">
+        <v>424</v>
+      </c>
+      <c r="C332" t="s">
         <v>425</v>
       </c>
-      <c r="C332" t="s">
+      <c r="D332" t="s">
         <v>426</v>
-      </c>
-      <c r="D332" t="s">
-        <v>427</v>
       </c>
       <c r="E332">
         <v>2</v>
@@ -25685,13 +25684,13 @@
         <v>216</v>
       </c>
       <c r="G332" t="s">
+        <v>427</v>
+      </c>
+      <c r="I332">
+        <v>1</v>
+      </c>
+      <c r="N332" t="s">
         <v>428</v>
-      </c>
-      <c r="I332">
-        <v>1</v>
-      </c>
-      <c r="N332" t="s">
-        <v>429</v>
       </c>
       <c r="P332">
         <v>10</v>
@@ -25732,16 +25731,16 @@
     </row>
     <row r="333" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B333" t="s">
+        <v>424</v>
+      </c>
+      <c r="C333" t="s">
         <v>425</v>
       </c>
-      <c r="C333" t="s">
+      <c r="D333" t="s">
         <v>426</v>
-      </c>
-      <c r="D333" t="s">
-        <v>427</v>
       </c>
       <c r="E333">
         <v>2</v>
@@ -25750,13 +25749,13 @@
         <v>269</v>
       </c>
       <c r="G333" t="s">
+        <v>429</v>
+      </c>
+      <c r="I333">
+        <v>1</v>
+      </c>
+      <c r="N333" t="s">
         <v>430</v>
-      </c>
-      <c r="I333">
-        <v>1</v>
-      </c>
-      <c r="N333" t="s">
-        <v>431</v>
       </c>
       <c r="P333">
         <v>8</v>
@@ -25791,16 +25790,16 @@
     </row>
     <row r="334" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B334" t="s">
+        <v>424</v>
+      </c>
+      <c r="C334" t="s">
         <v>425</v>
       </c>
-      <c r="C334" t="s">
+      <c r="D334" t="s">
         <v>426</v>
-      </c>
-      <c r="D334" t="s">
-        <v>427</v>
       </c>
       <c r="E334">
         <v>2</v>
@@ -25809,13 +25808,13 @@
         <v>107</v>
       </c>
       <c r="G334" t="s">
+        <v>431</v>
+      </c>
+      <c r="K334">
+        <v>1</v>
+      </c>
+      <c r="N334" t="s">
         <v>432</v>
-      </c>
-      <c r="K334">
-        <v>1</v>
-      </c>
-      <c r="N334" t="s">
-        <v>433</v>
       </c>
       <c r="P334">
         <v>4</v>
@@ -25838,16 +25837,16 @@
     </row>
     <row r="335" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B335" t="s">
+        <v>424</v>
+      </c>
+      <c r="C335" t="s">
         <v>425</v>
       </c>
-      <c r="C335" t="s">
+      <c r="D335" t="s">
         <v>426</v>
-      </c>
-      <c r="D335" t="s">
-        <v>427</v>
       </c>
       <c r="E335">
         <v>2</v>
@@ -25856,7 +25855,7 @@
         <v>359</v>
       </c>
       <c r="G335" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="K335">
         <v>1</v>
@@ -25865,7 +25864,7 @@
         <v>1</v>
       </c>
       <c r="N335" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="P335">
         <v>4</v>
@@ -25888,16 +25887,16 @@
     </row>
     <row r="336" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B336" t="s">
+        <v>424</v>
+      </c>
+      <c r="C336" t="s">
         <v>425</v>
       </c>
-      <c r="C336" t="s">
+      <c r="D336" t="s">
         <v>426</v>
-      </c>
-      <c r="D336" t="s">
-        <v>427</v>
       </c>
       <c r="E336">
         <v>2</v>
@@ -25906,7 +25905,7 @@
         <v>174</v>
       </c>
       <c r="G336" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H336">
         <v>1</v>
@@ -25929,16 +25928,16 @@
     </row>
     <row r="337" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B337" t="s">
+        <v>424</v>
+      </c>
+      <c r="C337" t="s">
         <v>425</v>
       </c>
-      <c r="C337" t="s">
+      <c r="D337" t="s">
         <v>426</v>
-      </c>
-      <c r="D337" t="s">
-        <v>427</v>
       </c>
       <c r="E337">
         <v>2</v>
@@ -25947,7 +25946,7 @@
         <v>124</v>
       </c>
       <c r="G337" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="J337">
         <v>1</v>
@@ -25956,7 +25955,7 @@
         <v>1</v>
       </c>
       <c r="N337" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="P337">
         <v>2</v>
@@ -25973,16 +25972,16 @@
     </row>
     <row r="338" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B338" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C338" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D338" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E338">
         <v>6</v>
@@ -25991,7 +25990,7 @@
         <v>248</v>
       </c>
       <c r="G338" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H338">
         <v>1</v>
@@ -26006,7 +26005,7 @@
         <v>1</v>
       </c>
       <c r="N338" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="P338">
         <v>10</v>
@@ -26047,16 +26046,16 @@
     </row>
     <row r="339" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B339" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C339" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D339" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E339">
         <v>6</v>
@@ -26065,7 +26064,7 @@
         <v>231</v>
       </c>
       <c r="G339" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="I339">
         <v>1</v>
@@ -26077,7 +26076,7 @@
         <v>1</v>
       </c>
       <c r="N339" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="P339">
         <v>8</v>
@@ -26112,16 +26111,16 @@
     </row>
     <row r="340" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B340" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C340" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D340" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E340">
         <v>6</v>
@@ -26130,13 +26129,13 @@
         <v>233</v>
       </c>
       <c r="G340" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H340">
         <v>1</v>
       </c>
       <c r="N340" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="P340">
         <v>10</v>
@@ -26177,16 +26176,16 @@
     </row>
     <row r="341" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B341" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C341" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D341" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E341">
         <v>6</v>
@@ -26195,7 +26194,7 @@
         <v>181</v>
       </c>
       <c r="G341" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="L341">
         <v>1</v>
@@ -26221,16 +26220,16 @@
     </row>
     <row r="342" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B342" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C342" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D342" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E342">
         <v>5</v>
@@ -26239,13 +26238,13 @@
         <v>210</v>
       </c>
       <c r="G342" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="K342">
         <v>1</v>
       </c>
       <c r="N342" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="P342">
         <v>8</v>
@@ -26280,16 +26279,16 @@
     </row>
     <row r="343" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B343" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C343" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D343" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E343">
         <v>5</v>
@@ -26298,13 +26297,13 @@
         <v>310</v>
       </c>
       <c r="G343" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="H343">
         <v>1</v>
       </c>
       <c r="N343" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="P343">
         <v>10</v>
@@ -26345,16 +26344,16 @@
     </row>
     <row r="344" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B344" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C344" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D344" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E344">
         <v>5</v>
@@ -26363,13 +26362,13 @@
         <v>143</v>
       </c>
       <c r="G344" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="H344">
         <v>1</v>
       </c>
       <c r="N344" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="P344">
         <v>10</v>
@@ -26410,16 +26409,16 @@
     </row>
     <row r="345" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B345" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C345" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D345" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E345">
         <v>5</v>
@@ -26428,7 +26427,7 @@
         <v>181</v>
       </c>
       <c r="G345" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="L345">
         <v>1</v>
@@ -26451,31 +26450,31 @@
     </row>
     <row r="346" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B346" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C346" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D346" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E346">
         <v>4</v>
       </c>
       <c r="F346" t="s">
+        <v>446</v>
+      </c>
+      <c r="G346" t="s">
         <v>447</v>
       </c>
-      <c r="G346" t="s">
-        <v>448</v>
-      </c>
       <c r="J346">
         <v>1</v>
       </c>
       <c r="N346" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="P346">
         <v>10</v>
@@ -26516,16 +26515,16 @@
     </row>
     <row r="347" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B347" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C347" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D347" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E347">
         <v>4</v>
@@ -26534,13 +26533,13 @@
         <v>207</v>
       </c>
       <c r="G347" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="J347">
         <v>1</v>
       </c>
       <c r="N347" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="P347">
         <v>8</v>
@@ -26575,16 +26574,16 @@
     </row>
     <row r="348" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B348" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C348" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D348" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E348">
         <v>4</v>
@@ -26593,13 +26592,13 @@
         <v>121</v>
       </c>
       <c r="G348" t="s">
+        <v>449</v>
+      </c>
+      <c r="H348">
+        <v>1</v>
+      </c>
+      <c r="N348" t="s">
         <v>450</v>
-      </c>
-      <c r="H348">
-        <v>1</v>
-      </c>
-      <c r="N348" t="s">
-        <v>451</v>
       </c>
       <c r="P348">
         <v>8</v>
@@ -26634,16 +26633,16 @@
     </row>
     <row r="349" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B349" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C349" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D349" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E349">
         <v>4</v>
@@ -26652,7 +26651,7 @@
         <v>137</v>
       </c>
       <c r="G349" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="L349">
         <v>1</v>
@@ -26675,16 +26674,16 @@
     </row>
     <row r="350" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B350" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C350" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D350" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E350">
         <v>4</v>
@@ -26693,7 +26692,7 @@
         <v>181</v>
       </c>
       <c r="G350" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="L350">
         <v>1</v>
@@ -26716,16 +26715,16 @@
     </row>
     <row r="351" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B351" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C351" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D351" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E351">
         <v>5</v>
@@ -26734,13 +26733,13 @@
         <v>210</v>
       </c>
       <c r="G351" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="K351">
         <v>1</v>
       </c>
       <c r="N351" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="P351">
         <v>8</v>
@@ -26775,16 +26774,16 @@
     </row>
     <row r="352" spans="1:90" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B352" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C352" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D352" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E352">
         <v>5</v>
@@ -26793,13 +26792,13 @@
         <v>310</v>
       </c>
       <c r="G352" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="H352">
         <v>1</v>
       </c>
       <c r="N352" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="P352">
         <v>4</v>
@@ -26822,16 +26821,16 @@
     </row>
     <row r="353" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B353" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C353" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D353" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E353">
         <v>5</v>
@@ -26840,13 +26839,13 @@
         <v>328</v>
       </c>
       <c r="G353" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="H353">
         <v>1</v>
       </c>
       <c r="N353" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="P353">
         <v>4</v>
@@ -26869,16 +26868,16 @@
     </row>
     <row r="354" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B354" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C354" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D354" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E354">
         <v>5</v>
@@ -26887,13 +26886,13 @@
         <v>143</v>
       </c>
       <c r="G354" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="H354">
         <v>1</v>
       </c>
       <c r="N354" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="P354">
         <v>10</v>
@@ -26934,16 +26933,16 @@
     </row>
     <row r="355" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B355" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C355" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D355" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E355">
         <v>5</v>
@@ -26952,13 +26951,13 @@
         <v>181</v>
       </c>
       <c r="G355" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="L355">
         <v>1</v>
       </c>
       <c r="N355" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="P355">
         <v>2</v>
@@ -26975,16 +26974,16 @@
     </row>
     <row r="356" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A356" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B356" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C356" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D356" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E356">
         <v>5</v>
@@ -26993,13 +26992,13 @@
         <v>163</v>
       </c>
       <c r="G356" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="J356">
         <v>1</v>
       </c>
       <c r="N356" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="P356">
         <v>2</v>
@@ -27016,16 +27015,16 @@
     </row>
     <row r="357" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B357" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C357" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D357" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E357">
         <v>1</v>
@@ -27034,13 +27033,13 @@
         <v>110</v>
       </c>
       <c r="G357" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="I357">
         <v>1</v>
       </c>
       <c r="N357" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="P357">
         <v>10</v>
@@ -27081,16 +27080,16 @@
     </row>
     <row r="358" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B358" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C358" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D358" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E358">
         <v>1</v>
@@ -27099,13 +27098,13 @@
         <v>272</v>
       </c>
       <c r="G358" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="M358">
         <v>1</v>
       </c>
       <c r="N358" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="P358">
         <v>8</v>
@@ -27140,16 +27139,16 @@
     </row>
     <row r="359" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B359" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C359" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D359" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E359">
         <v>1</v>
@@ -27158,7 +27157,7 @@
         <v>179</v>
       </c>
       <c r="G359" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="H359">
         <v>1</v>
@@ -27173,7 +27172,7 @@
         <v>1</v>
       </c>
       <c r="N359" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="P359">
         <v>8</v>
@@ -27208,16 +27207,16 @@
     </row>
     <row r="360" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A360" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B360" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C360" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D360" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E360">
         <v>1</v>
@@ -27226,7 +27225,7 @@
         <v>124</v>
       </c>
       <c r="G360" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H360">
         <v>1</v>
@@ -27252,16 +27251,16 @@
     </row>
     <row r="361" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B361" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C361" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D361" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E361">
         <v>1</v>
@@ -27270,13 +27269,13 @@
         <v>115</v>
       </c>
       <c r="G361" t="s">
+        <v>460</v>
+      </c>
+      <c r="I361">
+        <v>1</v>
+      </c>
+      <c r="N361" t="s">
         <v>461</v>
-      </c>
-      <c r="I361">
-        <v>1</v>
-      </c>
-      <c r="N361" t="s">
-        <v>462</v>
       </c>
       <c r="P361">
         <v>2</v>
@@ -27293,31 +27292,31 @@
     </row>
     <row r="362" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A362" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B362" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C362" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D362" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E362">
         <v>4</v>
       </c>
       <c r="F362" t="s">
+        <v>446</v>
+      </c>
+      <c r="G362" t="s">
         <v>447</v>
       </c>
-      <c r="G362" t="s">
-        <v>448</v>
-      </c>
       <c r="J362">
         <v>1</v>
       </c>
       <c r="N362" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="P362">
         <v>8</v>
@@ -27352,16 +27351,16 @@
     </row>
     <row r="363" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A363" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B363" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C363" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D363" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E363">
         <v>4</v>
@@ -27370,13 +27369,13 @@
         <v>207</v>
       </c>
       <c r="G363" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="J363">
         <v>1</v>
       </c>
       <c r="N363" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="P363">
         <v>10</v>
@@ -27417,16 +27416,16 @@
     </row>
     <row r="364" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A364" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B364" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C364" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D364" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E364">
         <v>4</v>
@@ -27435,13 +27434,13 @@
         <v>121</v>
       </c>
       <c r="G364" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="H364">
         <v>1</v>
       </c>
       <c r="N364" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="P364">
         <v>8</v>
@@ -27476,16 +27475,16 @@
     </row>
     <row r="365" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A365" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B365" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C365" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D365" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E365">
         <v>4</v>
@@ -27494,7 +27493,7 @@
         <v>137</v>
       </c>
       <c r="G365" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="L365">
         <v>1</v>
@@ -27517,16 +27516,16 @@
     </row>
     <row r="366" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A366" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B366" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C366" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D366" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E366">
         <v>4</v>
@@ -27535,7 +27534,7 @@
         <v>181</v>
       </c>
       <c r="G366" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="K366">
         <v>1</v>
@@ -27558,16 +27557,16 @@
     </row>
     <row r="367" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A367" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B367" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C367" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D367" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E367">
         <v>1</v>
@@ -27576,7 +27575,7 @@
         <v>179</v>
       </c>
       <c r="G367" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="H367">
         <v>1</v>
@@ -27591,7 +27590,7 @@
         <v>1</v>
       </c>
       <c r="N367" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P367">
         <v>8</v>
@@ -27626,16 +27625,16 @@
     </row>
     <row r="368" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A368" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B368" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C368" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D368" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E368">
         <v>1</v>
@@ -27644,13 +27643,13 @@
         <v>272</v>
       </c>
       <c r="G368" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="M368">
         <v>1</v>
       </c>
       <c r="N368" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P368">
         <v>8</v>
@@ -27685,16 +27684,16 @@
     </row>
     <row r="369" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A369" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B369" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C369" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D369" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E369">
         <v>1</v>
@@ -27703,13 +27702,13 @@
         <v>110</v>
       </c>
       <c r="G369" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="I369">
         <v>1</v>
       </c>
       <c r="N369" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="P369">
         <v>10</v>
@@ -27750,16 +27749,16 @@
     </row>
     <row r="370" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A370" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B370" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C370" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D370" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E370">
         <v>1</v>
@@ -27768,13 +27767,13 @@
         <v>115</v>
       </c>
       <c r="G370" t="s">
+        <v>460</v>
+      </c>
+      <c r="I370">
+        <v>1</v>
+      </c>
+      <c r="N370" t="s">
         <v>461</v>
-      </c>
-      <c r="I370">
-        <v>1</v>
-      </c>
-      <c r="N370" t="s">
-        <v>462</v>
       </c>
       <c r="P370">
         <v>2</v>
@@ -27791,16 +27790,16 @@
     </row>
     <row r="371" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A371" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B371" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C371" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D371" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E371">
         <v>1</v>
@@ -27809,7 +27808,7 @@
         <v>124</v>
       </c>
       <c r="G371" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H371">
         <v>1</v>
@@ -27835,16 +27834,16 @@
     </row>
     <row r="372" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A372" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B372" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C372" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D372" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E372">
         <v>1</v>
@@ -27853,16 +27852,16 @@
         <v>110</v>
       </c>
       <c r="G372" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="I372">
         <v>1</v>
       </c>
       <c r="N372" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="P372">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="Q372">
         <v>96</v>
@@ -27891,19 +27890,25 @@
       <c r="BU372">
         <v>1004</v>
       </c>
+      <c r="CN372">
+        <v>1004</v>
+      </c>
+      <c r="CO372">
+        <v>1004</v>
+      </c>
     </row>
     <row r="373" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A373" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B373" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C373" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D373" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E373">
         <v>1</v>
@@ -27912,13 +27917,13 @@
         <v>272</v>
       </c>
       <c r="G373" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="M373">
         <v>1</v>
       </c>
       <c r="N373" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P373">
         <v>8</v>
@@ -27953,16 +27958,16 @@
     </row>
     <row r="374" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A374" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B374" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C374" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D374" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E374">
         <v>1</v>
@@ -27971,7 +27976,7 @@
         <v>179</v>
       </c>
       <c r="G374" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="H374">
         <v>1</v>
@@ -27986,7 +27991,7 @@
         <v>1</v>
       </c>
       <c r="N374" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P374">
         <v>6</v>
@@ -28015,16 +28020,16 @@
     </row>
     <row r="375" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A375" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B375" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C375" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D375" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E375">
         <v>1</v>
@@ -28033,13 +28038,13 @@
         <v>115</v>
       </c>
       <c r="G375" t="s">
+        <v>460</v>
+      </c>
+      <c r="J375">
+        <v>1</v>
+      </c>
+      <c r="N375" t="s">
         <v>461</v>
-      </c>
-      <c r="J375">
-        <v>1</v>
-      </c>
-      <c r="N375" t="s">
-        <v>462</v>
       </c>
       <c r="P375">
         <v>2</v>
@@ -28056,16 +28061,16 @@
     </row>
     <row r="376" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A376" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B376" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C376" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D376" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E376">
         <v>1</v>
@@ -28074,7 +28079,7 @@
         <v>174</v>
       </c>
       <c r="G376" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="I376">
         <v>1</v>
@@ -28097,16 +28102,16 @@
     </row>
     <row r="377" spans="1:105" x14ac:dyDescent="0.3">
       <c r="A377" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B377" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C377" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D377" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E377">
         <v>1</v>
@@ -28115,7 +28120,7 @@
         <v>124</v>
       </c>
       <c r="G377" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H377">
         <v>1</v>
@@ -28124,7 +28129,7 @@
         <v>1</v>
       </c>
       <c r="N377" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="P377">
         <v>2</v>
@@ -28438,11 +28443,11 @@
       </c>
       <c r="CN378">
         <f>SUBTOTAL(3,PROGRAMACIONES_PARCIALES[16-17V])</f>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="CO378">
         <f>SUBTOTAL(3,PROGRAMACIONES_PARCIALES[17-18V])</f>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="CP378">
         <f>SUBTOTAL(3,PROGRAMACIONES_PARCIALES[18-19V])</f>
@@ -28546,10 +28551,10 @@
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B3" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -28586,7 +28591,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B8">
         <v>30</v>
@@ -28602,7 +28607,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B10">
         <v>34</v>
@@ -28618,7 +28623,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B12">
         <v>30</v>
@@ -28634,7 +28639,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B14">
         <v>26</v>
@@ -28650,7 +28655,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B16">
         <v>18</v>
@@ -28666,7 +28671,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B18">
         <v>14</v>
@@ -28682,7 +28687,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B20">
         <v>24</v>
@@ -28690,7 +28695,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B21">
         <v>34</v>
@@ -28698,7 +28703,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B22">
         <v>32</v>
@@ -28730,7 +28735,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B26">
         <v>24</v>
@@ -28738,7 +28743,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B27">
         <v>24</v>
@@ -28746,7 +28751,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B28">
         <v>24</v>
@@ -28754,7 +28759,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B29">
         <v>25</v>
@@ -28768,10 +28773,10 @@
         <v>24</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E30" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -28796,7 +28801,7 @@
         <v>36</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E32">
         <v>1</v>
@@ -28810,7 +28815,7 @@
         <v>30</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E33">
         <v>9</v>
@@ -28838,7 +28843,7 @@
         <v>28</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E35">
         <v>1</v>
@@ -28916,13 +28921,13 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B41">
         <v>26</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E41">
         <v>1</v>
@@ -29006,7 +29011,7 @@
         <v>22</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E47">
         <v>69</v>
@@ -29046,7 +29051,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B52">
         <v>22</v>
@@ -29054,7 +29059,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B53">
         <v>38</v>
@@ -29118,7 +29123,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B61">
         <v>26</v>
@@ -29126,7 +29131,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B62">
         <v>22</v>
@@ -29158,7 +29163,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B66">
         <v>26</v>
@@ -29174,7 +29179,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B68">
         <v>30</v>
@@ -29182,7 +29187,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="4" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B69">
         <v>10</v>
@@ -29222,7 +29227,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B74">
         <v>34</v>
@@ -29246,7 +29251,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B77">
         <v>26</v>
@@ -29286,7 +29291,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="4" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B82">
         <v>2042</v>

</xml_diff>